<commit_message>
Changed AI checkpoint to look for a check_mark instead of a check_box to have it look for the check mark that shows up when submitting the order is successful
</commit_message>
<xml_diff>
--- a/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
+++ b/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
@@ -208,7 +208,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -222,6 +222,26 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -244,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -252,9 +272,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,17 +589,17 @@
     <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" customFormat="1">
-      <c r="A1" t="s">
+    <row r="1" ht="14.95" s="6" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -590,7 +613,7 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -692,17 +715,17 @@
     <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" customFormat="1">
-      <c r="A1" t="s">
+    <row r="1" ht="14.95" s="6" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -716,7 +739,7 @@
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added vl01n tcode to the process to create an outbound delivery document for the order
</commit_message>
<xml_diff>
--- a/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
+++ b/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -16,13 +16,17 @@
     <sheet name="07_va01_exit" sheetId="7" r:id="rId7"/>
     <sheet name="99_logout" sheetId="8" r:id="rId8"/>
     <sheet name="06_va01_create_new_order" sheetId="9" r:id="rId9"/>
+    <sheet name="08_Launch_TCode_vl01n" sheetId="10" r:id="rId10"/>
+    <sheet name="09_vl01n_create_outbound_de..00" sheetId="11" r:id="rId11"/>
+    <sheet name="10_vl01n_outbound_delivery_..00" sheetId="12" r:id="rId12"/>
+    <sheet name="11_vl01n_exit" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>BrowserName</t>
   </si>
@@ -30,6 +34,9 @@
     <t>https://sap-hana.mfdemoportal.com:44300/sap/bc/ui2/flp?sap-client=100&amp;sap-language=EN#Shell-home</t>
   </si>
   <si>
+    <t>OrderNumber</t>
+  </si>
+  <si>
     <t>CHROME</t>
   </si>
   <si>
@@ -64,6 +71,9 @@
   </si>
   <si>
     <t>URL</t>
+  </si>
+  <si>
+    <t>DeliveryNumber</t>
   </si>
 </sst>
 </file>
@@ -273,11 +283,11 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -586,37 +596,122 @@
     <col min="2" max="2" width="86.47265625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.34375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="14.95" s="6" customFormat="1">
+    <col min="5" max="6" width="9.41796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="6"/>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -715,18 +810,18 @@
     <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="6" customFormat="1">
+    <row r="1" ht="14.95" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2">
@@ -734,13 +829,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>4</v>
+      <c r="D2" s="6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -790,7 +885,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added additional steps to get through post goods issue, currently something wrong in the system preventing from moving further.
</commit_message>
<xml_diff>
--- a/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
+++ b/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="12"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="09_vl01n_create_outbound_de..00" sheetId="11" r:id="rId11"/>
     <sheet name="10_vl01n_outbound_delivery_..00" sheetId="12" r:id="rId12"/>
     <sheet name="11_vl01n_exit" sheetId="13" r:id="rId13"/>
+    <sheet name="12_Launch_TCode_vl02n" sheetId="14" r:id="rId14"/>
+    <sheet name="13_change_outbound_delivery" sheetId="15" r:id="rId15"/>
+    <sheet name="14_change_outbound_delivery..00" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
@@ -587,7 +590,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -596,7 +599,8 @@
     <col min="2" max="2" width="86.47265625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.34375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7890625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.41796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.65234375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -702,6 +706,63 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -798,7 +859,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>

</xml_diff>

<commit_message>
Completing OTC process, create sales order, create delivery, create billing doc, post receipt of funds
</commit_message>
<xml_diff>
--- a/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
+++ b/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="SpreadsheetGear 8.2.5.102"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="15"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18075" windowHeight="9900" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
@@ -23,13 +23,17 @@
     <sheet name="12_Launch_TCode_vl02n" sheetId="14" r:id="rId14"/>
     <sheet name="13_change_outbound_delivery" sheetId="15" r:id="rId15"/>
     <sheet name="14_change_outbound_delivery..00" sheetId="16" r:id="rId16"/>
+    <sheet name="15_Launch_TCode_vf01" sheetId="17" r:id="rId17"/>
+    <sheet name="16_vf01_create_billing_document" sheetId="18" r:id="rId18"/>
+    <sheet name="17_Nav_to_Post_Incoming_Pay..00" sheetId="19" r:id="rId19"/>
+    <sheet name="18_Post_Incoming_Payments" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="40001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>BrowserName</t>
   </si>
@@ -40,6 +44,9 @@
     <t>OrderNumber</t>
   </si>
   <si>
+    <t>DocumentNumber</t>
+  </si>
+  <si>
     <t>CHROME</t>
   </si>
   <si>
@@ -53,6 +60,9 @@
   </si>
   <si>
     <t>s4h_sd_dem</t>
+  </si>
+  <si>
+    <t>BillingNumber</t>
   </si>
   <si>
     <t>EWMS4-02</t>
@@ -254,7 +264,9 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -265,9 +277,7 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -286,11 +296,11 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -601,44 +611,54 @@
     <col min="4" max="4" width="9.7890625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.671875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.65234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.078125" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="14.95" s="4" customFormat="1">
+    <col min="7" max="7" width="12.921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.4140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" s="6" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>15</v>
+      <c r="F1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="6"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -734,23 +754,118 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
-  <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.95"/>
+  <cols>
+    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>
@@ -759,7 +874,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -778,25 +893,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
-  <cols>
-    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
@@ -859,7 +955,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -871,18 +967,18 @@
     <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="4" customFormat="1">
+    <row r="1" ht="14.95" s="6" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2">
@@ -890,13 +986,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>5</v>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to allow parameter driving from MBT instead of data table, will use datatable values if MBT doesn't pass the correct values, only the default values.
</commit_message>
<xml_diff>
--- a/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
+++ b/uft-one-ai-sap-fiori-va01-s4hana/Default.xlsx
@@ -242,9 +242,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -253,7 +251,9 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -292,15 +292,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,7 +600,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -616,49 +616,49 @@
     <col min="9" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="6" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="14.95" s="4" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="4"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -849,31 +849,31 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="14.95" customFormat="1"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.95"/>
+  <cols>
+    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.95"/>
-  <cols>
-    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="1"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
@@ -887,7 +887,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -967,31 +967,31 @@
     <col min="5" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" s="6" customFormat="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" ht="14.95" s="4" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>